<commit_message>
por eso BadBuny ni ronca
</commit_message>
<xml_diff>
--- a/Proyectos/proyectoCredito/Documentacion/PJ CREDITO.xlsx
+++ b/Proyectos/proyectoCredito/Documentacion/PJ CREDITO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PERSONAL\Proyectos\proyectoCredito\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC49FC0-913A-4A46-820D-C41F161F0903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68FB2AD-4044-4185-AD3E-BE2C5BA7809D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1CB0A026-64F2-48AC-B9D8-8682899DB3CB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>REQUERIMIENTOS</t>
   </si>
@@ -87,9 +87,6 @@
     <t>MONTO_DEUDA</t>
   </si>
   <si>
-    <t>FECHA_DEUDA</t>
-  </si>
-  <si>
     <t>CLAVE_USUARIO</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>MONTO_PAGO</t>
   </si>
   <si>
-    <t>FECHA_PAGO</t>
-  </si>
-  <si>
     <t>CUOTA_DEUDA</t>
   </si>
   <si>
@@ -151,6 +145,18 @@
   </si>
   <si>
     <t>DNI_DEUDOR</t>
+  </si>
+  <si>
+    <t>FECHAACT_PAGO</t>
+  </si>
+  <si>
+    <t>FECHAREG_PAGO</t>
+  </si>
+  <si>
+    <t>FECHAREG_DEUDA</t>
+  </si>
+  <si>
+    <t>FECHAACT_DEUDA</t>
   </si>
 </sst>
 </file>
@@ -227,14 +233,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,10 +634,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D220C0-6FDB-4206-A87C-09947B373F4C}">
-  <dimension ref="B3:J22"/>
+  <dimension ref="B3:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,110 +645,117 @@
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
       <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="3" t="s">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>36</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -762,23 +774,23 @@
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
         <v>20</v>
-      </c>
-      <c r="C22" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>